<commit_message>
Inserted kNN to chart
</commit_message>
<xml_diff>
--- a/Algorithm Metrics.xlsx
+++ b/Algorithm Metrics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2547fb8ee856ab20/Desktop/DSProject-Flights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galha\Downloads\לימודים\שנה ב\יסודות מדעי הנתונים\DSProject-Flights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69CDDD5C-DE0B-4DDC-9048-F0DD7C16E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65C7790-1C8B-4D7F-A239-7EE357722E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>R2</t>
   </si>
@@ -52,6 +52,9 @@
   <si>
     <t>algo</t>
   </si>
+  <si>
+    <t>kNN</t>
+  </si>
 </sst>
 </file>
 
@@ -61,7 +64,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -125,7 +128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,15 +447,15 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -469,56 +472,66 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="C2" s="1">
+        <v>58.08</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6760.02</v>
+      </c>
+      <c r="E2" s="1">
+        <v>82.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>

</xml_diff>

<commit_message>
site compare deceission tree
</commit_message>
<xml_diff>
--- a/Algorithm Metrics.xlsx
+++ b/Algorithm Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2547fb8ee856ab20/Desktop/DSProject-Flights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{69CDDD5C-DE0B-4DDC-9048-F0DD7C16E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3968652F-06EF-4BAA-BC65-BB4A5A24279A}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{69CDDD5C-DE0B-4DDC-9048-F0DD7C16E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD5F8A0A-C7F9-449A-A9DD-309E876510AC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>R2</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>Decision Tree Regressor</t>
+  </si>
+  <si>
+    <t>גל</t>
+  </si>
+  <si>
+    <t>טלנ</t>
+  </si>
+  <si>
+    <t>אנדריי</t>
   </si>
 </sst>
 </file>
@@ -129,40 +138,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -217,44 +193,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -266,6 +204,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -585,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0432AB5-8137-4B7B-A00C-3EEFAD33DCF0}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -600,7 +542,7 @@
     <col min="5" max="5" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -617,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -634,7 +576,7 @@
         <v>80.38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -651,65 +593,83 @@
         <v>82.07</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D9">
+    <cfRule type="top10" dxfId="2" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E9">
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>MAX($B$2:$B$9)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B9">
-    <cfRule type="top10" dxfId="7" priority="4" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C9">
-    <cfRule type="top10" dxfId="6" priority="3" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9">
-    <cfRule type="top10" dxfId="5" priority="2" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9">
-    <cfRule type="top10" dxfId="4" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Inserted my algo scores
</commit_message>
<xml_diff>
--- a/Algorithm Metrics.xlsx
+++ b/Algorithm Metrics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2547fb8ee856ab20/Desktop/DSProject-Flights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galha\Downloads\לימודים\שנה ב\יסודות מדעי הנתונים\DSProject-Flights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{69CDDD5C-DE0B-4DDC-9048-F0DD7C16E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD5F8A0A-C7F9-449A-A9DD-309E876510AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0039151B-0A6E-4867-8024-1BC0190725AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>R2</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>אנדריי</t>
+  </si>
+  <si>
+    <t>Support Vector Regressor</t>
+  </si>
+  <si>
+    <t>K Nearest Neighbors</t>
   </si>
 </sst>
 </file>
@@ -76,7 +82,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -138,7 +144,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -206,12 +223,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -530,19 +543,19 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.8984375" customWidth="1"/>
-    <col min="2" max="2" width="12.09765625" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="4" max="4" width="12.296875" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" customWidth="1"/>
+    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -559,61 +572,81 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>0.84950000000000003</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>57.85</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>6460.3</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>80.38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>0.84309999999999996</v>
       </c>
       <c r="C3" s="4">
         <v>58.73</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>6735.38</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>82.07</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.2636</v>
+      </c>
+      <c r="C4" s="2">
+        <v>129.03</v>
+      </c>
+      <c r="D4" s="2">
+        <v>31605.17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>177.78</v>
+      </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.8458</v>
+      </c>
+      <c r="C5" s="2">
+        <v>57.624200000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6619.5820000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>81.360799999999998</v>
+      </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -623,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -633,7 +666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -643,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -655,21 +688,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B9">
-    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C9">
+  <conditionalFormatting sqref="C6:C9">
+    <cfRule type="top10" dxfId="4" priority="4" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3 D6:D9">
     <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="E2:E3 E6:E9">
     <cfRule type="top10" dxfId="2" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9">
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>MAX($B$2:$B$9)</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Word & Updated Algo Metrics
</commit_message>
<xml_diff>
--- a/Algorithm Metrics.xlsx
+++ b/Algorithm Metrics.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2547fb8ee856ab20/Desktop/DSProject-Flights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\Desktop\Andrian\DSProject-Flights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{0039151B-0A6E-4867-8024-1BC0190725AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E112950-27B6-4B59-880B-7D8C56DE1A39}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E5BAA9-B743-4EB4-AEC4-4B0D4464FF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{55B23624-3FAF-4EFD-91FD-2E53BABFA757}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>R2</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>K Nearest Neighbors</t>
+  </si>
+  <si>
+    <t>XGBOOST</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -151,244 +154,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -769,19 +534,19 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.8984375" customWidth="1"/>
-    <col min="2" max="2" width="12.09765625" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" customWidth="1"/>
-    <col min="5" max="5" width="11.8984375" customWidth="1"/>
+    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -798,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -815,7 +580,7 @@
         <v>80.38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -832,7 +597,7 @@
         <v>82.07</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -852,7 +617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -872,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -882,7 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -892,17 +657,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.90369999999999995</v>
+      </c>
+      <c r="C8" s="3">
+        <v>47.14</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4133.21</v>
+      </c>
+      <c r="E8" s="3">
+        <v>64.290000000000006</v>
+      </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -914,19 +689,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B9">
-    <cfRule type="top10" dxfId="9" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="top10" dxfId="8" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D9">
-    <cfRule type="top10" dxfId="7" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E9">
-    <cfRule type="top10" dxfId="6" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>MAX($B$2:$B$9)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>